<commit_message>
Add links to printed parts on Etsy.
</commit_message>
<xml_diff>
--- a/Modules/CVMod8/CVMod8_BOM.xlsx
+++ b/Modules/CVMod8/CVMod8_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
   <si>
     <t>Qty</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005003256254825.html</t>
+  </si>
+  <si>
+    <t>https://avalonharmonics.etsy.com/listing/1641852285/printed-parts-avalon-harmonics-cvmod8</t>
+  </si>
+  <si>
+    <t>Purchase in Etsy Store:</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1231,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,12 +1707,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1715,6 +1722,12 @@
       </c>
       <c r="C34" s="3" t="s">
         <v>91</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1740,8 +1753,9 @@
     <hyperlink ref="F24" r:id="rId19"/>
     <hyperlink ref="F25" r:id="rId20"/>
     <hyperlink ref="L5" r:id="rId21"/>
+    <hyperlink ref="F34" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CVMod8 BOM for new slider pot source.
</commit_message>
<xml_diff>
--- a/Modules/CVMod8/CVMod8_BOM.xlsx
+++ b/Modules/CVMod8/CVMod8_BOM.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\CVMod8\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC32951E-E561-41E5-BD73-346E33B65EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CVMod8" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -164,9 +183,6 @@
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/befaco-parts/</t>
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/l-937egw/tht-leds-3mm/kingbright-electronic/</t>
@@ -351,11 +367,14 @@
   <si>
     <t>Purchase in Etsy Store:</t>
   </si>
+  <si>
+    <t>https://shop.befaco.org/potentiometers/282-30mm-faderslider-potentiometer-b100k-x4-units.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -937,14 +956,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -982,7 +1004,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1054,7 +1076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1227,11 +1249,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,7 +1304,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1302,7 +1324,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1322,7 +1344,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1342,10 +1364,10 @@
         <v>27</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1365,7 +1387,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,7 +1407,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1405,7 +1427,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,7 +1447,7 @@
         <v>46</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1445,7 +1467,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1462,10 +1484,10 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1485,7 +1507,7 @@
         <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1505,7 +1527,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1513,10 +1535,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>30</v>
@@ -1525,7 +1547,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1533,13 +1555,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -1550,13 +1572,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -1567,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -1584,16 +1606,16 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1604,16 +1626,16 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1621,16 +1643,16 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1638,16 +1660,16 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1655,16 +1677,16 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
       </c>
-      <c r="E24" t="s">
-        <v>70</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,16 +1694,16 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
         <v>77</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1694,22 +1716,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1718,42 +1740,42 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1"/>
-    <hyperlink ref="F13" r:id="rId2"/>
-    <hyperlink ref="F14" r:id="rId3"/>
-    <hyperlink ref="F11" r:id="rId4"/>
-    <hyperlink ref="F10" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
-    <hyperlink ref="F6" r:id="rId8"/>
-    <hyperlink ref="F5" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="F4" r:id="rId11"/>
-    <hyperlink ref="F3" r:id="rId12"/>
-    <hyperlink ref="F2" r:id="rId13"/>
-    <hyperlink ref="F23" r:id="rId14"/>
-    <hyperlink ref="C34" r:id="rId15"/>
-    <hyperlink ref="F19" r:id="rId16"/>
-    <hyperlink ref="F21" r:id="rId17"/>
-    <hyperlink ref="F22" r:id="rId18"/>
-    <hyperlink ref="F24" r:id="rId19"/>
-    <hyperlink ref="F25" r:id="rId20"/>
-    <hyperlink ref="L5" r:id="rId21"/>
-    <hyperlink ref="F34" r:id="rId22"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F2" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C34" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L5" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>

</xml_diff>

<commit_message>
Clarify isolated resistor array.
</commit_message>
<xml_diff>
--- a/Modules/CVMod8/CVMod8_BOM.xlsx
+++ b/Modules/CVMod8/CVMod8_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\CVMod8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC32951E-E561-41E5-BD73-346E33B65EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E8A1E4-A622-4691-A638-1253446C02B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>Resistor THT</t>
   </si>
   <si>
-    <t>Resistor Network THT, 4 Split Resistors</t>
-  </si>
-  <si>
     <t>DIP-14</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>https://shop.befaco.org/potentiometers/282-30mm-faderslider-potentiometer-b100k-x4-units.html</t>
+  </si>
+  <si>
+    <t>Resistor Network THT, 4 Isolated Resistors</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="107.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1283,7 +1283,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1304,7 +1304,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1361,13 +1361,13 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1378,16 +1378,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1398,16 +1398,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1418,16 +1418,16 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1435,19 +1435,19 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,16 +1458,16 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,16 +1478,16 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1498,16 +1498,16 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1515,19 +1515,19 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1535,19 +1535,19 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1555,16 +1555,16 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1572,16 +1572,16 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1606,16 +1606,16 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
         <v>86</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E19" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1626,16 +1626,16 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="E21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1643,16 +1643,16 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1660,16 +1660,16 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,16 +1677,16 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
         <v>68</v>
       </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1694,21 +1694,21 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
         <v>76</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1716,22 +1716,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1740,16 +1740,16 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all BOMs to include a source for single row headers.
</commit_message>
<xml_diff>
--- a/Modules/CVMod8/CVMod8_BOM.xlsx
+++ b/Modules/CVMod8/CVMod8_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\CVMod8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E8A1E4-A622-4691-A638-1253446C02B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9D1CFC-9381-444B-9B9F-03CED57DFA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
   <si>
     <t>Qty</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>Resistor Network THT, 4 Isolated Resistors</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1256,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,6 +1569,9 @@
       <c r="E15" t="s">
         <v>32</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1582,6 +1588,9 @@
       </c>
       <c r="E16" t="s">
         <v>32</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,8 +1785,9 @@
     <hyperlink ref="F25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="L5" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="F34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F15:F16" r:id="rId23" display="https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/" xr:uid="{5FADD932-BCFE-4359-9848-C49990507EC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update all BOMs with a link to a 2x5 power header.
</commit_message>
<xml_diff>
--- a/Modules/CVMod8/CVMod8_BOM.xlsx
+++ b/Modules/CVMod8/CVMod8_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\CVMod8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9D1CFC-9381-444B-9B9F-03CED57DFA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA327669-2840-4641-A1EF-E28BF959CBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
   <si>
     <t>Qty</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/zl202-80g/pin-headers/connfly/ds1021-2-40sf11/</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1259,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,6 +1611,9 @@
       </c>
       <c r="E17" t="s">
         <v>32</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1786,8 +1792,9 @@
     <hyperlink ref="L5" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="F34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="F15:F16" r:id="rId23" display="https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/" xr:uid="{5FADD932-BCFE-4359-9848-C49990507EC0}"/>
+    <hyperlink ref="F17" r:id="rId24" xr:uid="{602FB34B-4263-4C36-BC2D-81826C90FB25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>